<commit_message>
Adição de tarefa no toDo Commit Diagrama ER
</commit_message>
<xml_diff>
--- a/tcc/docs/toDo.xlsx
+++ b/tcc/docs/toDo.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\313004\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\313004\git\repository\tcc\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="40">
   <si>
     <t>Descrição</t>
   </si>
@@ -142,6 +142,9 @@
   </si>
   <si>
     <t>Controle de envio e resposta -&gt; Adicionar campos Enviado e Resppondido na tabela AVALIACAO</t>
+  </si>
+  <si>
+    <t>Corrigir alinhamento botões editar/excluir das tabelas</t>
   </si>
 </sst>
 </file>
@@ -183,7 +186,7 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -204,21 +207,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -233,50 +222,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -574,10 +519,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D29"/>
+  <dimension ref="A1:D30"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -994,15 +939,29 @@
         <v>36</v>
       </c>
     </row>
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" t="s">
+        <v>26</v>
+      </c>
+      <c r="D30" t="s">
+        <v>36</v>
+      </c>
+    </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D180">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Waiting"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Atualização do Arquivo toDo.xlsx
- Tarefas em Progresso:
	01 - Remover relacionamento da tabela AVALIACAO com a tabela TURMA
	02 - Remover relacionamento da tabela AVALIACAO com a tabela ALUNO
	03 - Criar relacionamentoda tabela AVALIACAO com TURMA_X_ALUNO
	26 - Abertura de avaliação
</commit_message>
<xml_diff>
--- a/tcc/docs/toDo.xlsx
+++ b/tcc/docs/toDo.xlsx
@@ -1,21 +1,18 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="153222"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\313004\Desktop\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20325"/>
+  <workbookPr/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:801_{251D95ED-3BC1-48A4-9454-08112F0638AE}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="15000" windowHeight="6780" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -147,9 +144,17 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -177,13 +182,14 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="8">
+  <dxfs count="3">
     <dxf>
       <font>
         <b/>
@@ -204,21 +210,7 @@
       </font>
       <fill>
         <patternFill>
-          <bgColor rgb="FFFFC000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <strike val="0"/>
-        <u val="none"/>
-        <color theme="0"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
+          <bgColor theme="7" tint="0.39994506668294322"/>
         </patternFill>
       </fill>
     </dxf>
@@ -233,50 +225,6 @@
       <fill>
         <patternFill>
           <bgColor rgb="FFFF5050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="5"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor theme="7" tint="0.39994506668294322"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <b/>
-        <i val="0"/>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FF92D050"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <font>
-        <color rgb="FFFF0000"/>
-      </font>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFF0000"/>
         </patternFill>
       </fill>
     </dxf>
@@ -299,13 +247,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Table1" displayName="Table1" ref="A1:D180" totalsRowShown="0">
-  <autoFilter ref="A1:D180"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table1" displayName="Table1" ref="A1:D180" totalsRowShown="0">
+  <autoFilter ref="A1:D180" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
   <tableColumns count="4">
-    <tableColumn id="1" name="Codigo"/>
-    <tableColumn id="2" name="Descrição"/>
-    <tableColumn id="3" name="Responsável"/>
-    <tableColumn id="4" name="Status"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="Codigo"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="Descrição"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="Responsável"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="Status"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -573,11 +521,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="F3" sqref="F3"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -613,7 +561,7 @@
         <v>31</v>
       </c>
       <c r="D2" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -627,7 +575,7 @@
         <v>31</v>
       </c>
       <c r="D3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -641,7 +589,7 @@
         <v>31</v>
       </c>
       <c r="D4" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -718,7 +666,7 @@
       <c r="A10">
         <v>9</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="1" t="s">
         <v>9</v>
       </c>
       <c r="C10" t="s">
@@ -963,7 +911,7 @@
         <v>31</v>
       </c>
       <c r="D27" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="28" spans="1:4" x14ac:dyDescent="0.25">
@@ -996,25 +944,25 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="D2:D180">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="3" operator="equal">
       <formula>"Waiting"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="2" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
       <formula>"In Progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="1" operator="equal">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
       <formula>"Closed"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="360" r:id="rId1"/>
   <tableParts count="1">
     <tablePart r:id="rId2"/>
   </tableParts>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{CCE6A557-97BC-4b89-ADB6-D9C93CAAB3DF}">
       <x14:dataValidations xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" count="1">
-        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1">
+        <x14:dataValidation type="list" allowBlank="1" showInputMessage="1" showErrorMessage="1" xr:uid="{00000000-0002-0000-0000-000000000000}">
           <x14:formula1>
             <xm:f>Sheet2!$A$2:$A$5</xm:f>
           </x14:formula1>
@@ -1027,7 +975,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>